<commit_message>
Wyłączenie funkcjonalności zapisywania pliku Excel, przebudowanie aplikacji do współpracy z bazą danych i dodanie prostego menu z logowaniem.
</commit_message>
<xml_diff>
--- a/Character_data.xlsx
+++ b/Character_data.xlsx
@@ -65,34 +65,34 @@
     <t>Height</t>
   </si>
   <si>
-    <t>175 cm (5'9")</t>
-  </si>
-  <si>
-    <t>60 cm(2')</t>
-  </si>
-  <si>
-    <t>170 cm (5'7")</t>
-  </si>
-  <si>
-    <t>165 cm (5'5")</t>
-  </si>
-  <si>
-    <t>181 cm (5'11")</t>
-  </si>
-  <si>
-    <t>164 cm (5'5")</t>
-  </si>
-  <si>
-    <t>152 cm (5'0")</t>
-  </si>
-  <si>
-    <t>158 cm (5'2")</t>
-  </si>
-  <si>
-    <t>178 cm (5'10")</t>
-  </si>
-  <si>
-    <t>162 cm (5'4")</t>
+    <t>175cm</t>
+  </si>
+  <si>
+    <t>60cm</t>
+  </si>
+  <si>
+    <t>170cm</t>
+  </si>
+  <si>
+    <t>165cm</t>
+  </si>
+  <si>
+    <t>181cm</t>
+  </si>
+  <si>
+    <t>164cm</t>
+  </si>
+  <si>
+    <t>152cm</t>
+  </si>
+  <si>
+    <t>158cm</t>
+  </si>
+  <si>
+    <t>178cm</t>
+  </si>
+  <si>
+    <t>162cm</t>
   </si>
   <si>
     <t>Arcana</t>
@@ -209,7 +209,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="12.99609375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.4140625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.0234375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.84375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="17.0703125" customWidth="true" bestFit="true"/>

</xml_diff>